<commit_message>
delete kpi pdf page 3
</commit_message>
<xml_diff>
--- a/excels/Form 5 - KPI HSSE.xlsx
+++ b/excels/Form 5 - KPI HSSE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/ecsms/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68963C40-9A54-B34D-902A-2ABB61010EE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7322145-663A-B14F-8C3A-04A773AB6DD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{5302258C-DE74-E84C-B3AC-298106201E44}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t>EVALUASI PENCAPAIAN HSE PERFORMANCE INDICATOR</t>
   </si>
@@ -189,137 +189,10 @@
     <t xml:space="preserve">% TOTAL NILAI = </t>
   </si>
   <si>
-    <t>Lagging Indicator :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Score Actual = </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     x 100%</t>
-  </si>
-  <si>
-    <t>Leading Indicator :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% Total Nilai = </t>
-  </si>
-  <si>
-    <t>Ditandatangani Oleh :</t>
-  </si>
-  <si>
-    <t>……………………………………….</t>
-  </si>
-  <si>
-    <t>……………………………………………</t>
-  </si>
-  <si>
-    <t>………………………………………………</t>
-  </si>
-  <si>
-    <t>…………………………………………………</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOTE : </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Approval </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Pusat</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> &amp;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Region </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>: Wakil Fungsi HSSE (sesuai organisasi proyek) &amp; Direksi Pekerjaan</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Approval</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Lokasi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> : Spv HSSE &amp; Direksi Pekerjaan</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Region Manager HSSE MOR IV</t>
-  </si>
-  <si>
-    <t>I Made Dwi Darmaputra</t>
-  </si>
-  <si>
-    <t>Region Manager Aviation IV</t>
-  </si>
-  <si>
-    <t>Agus Sujatmoko</t>
-  </si>
-  <si>
-    <t>Σ [pencapaian actual untuk masing-masing indicator]</t>
-  </si>
-  <si>
-    <t>Σ [target yang ditentukan dari masing-masing item indicator]</t>
-  </si>
-  <si>
-    <t>Σ [target - [pencapaian actual untuk masing-masing indicator]]</t>
-  </si>
-  <si>
-    <t>Jumlah score actual yang dicapai terhadap seluruh item indicator</t>
-  </si>
-  <si>
-    <t>Jumlah Score maksimum dari seluruh item yang ditetapkan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
+    <t>placeholder-for-three-signs</t>
   </si>
 </sst>
 </file>
@@ -442,7 +315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -575,29 +448,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -682,13 +537,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -698,6 +547,99 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -705,107 +647,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1183,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F21146-6FE8-1A49-8795-7C0553228E43}">
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1217,17 +1069,17 @@
       <c r="M1" s="10"/>
     </row>
     <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.15">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
@@ -1235,7 +1087,7 @@
     </row>
     <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -1251,76 +1103,76 @@
       <c r="M3" s="10"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="45" t="s">
+      <c r="B4" s="64"/>
+      <c r="C4" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="45" t="s">
+      <c r="B5" s="64"/>
+      <c r="C5" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="45" t="s">
+      <c r="B6" s="64"/>
+      <c r="C6" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="45" t="s">
+      <c r="B7" s="64"/>
+      <c r="C7" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
@@ -1328,7 +1180,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -1347,10 +1199,10 @@
       <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="42"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="14" t="s">
         <v>9</v>
       </c>
@@ -1370,24 +1222,24 @@
         <v>14</v>
       </c>
       <c r="J9" s="16"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
     </row>
     <row r="10" spans="1:13" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>1</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="43"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="44" t="s">
+      <c r="F10" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="44" t="s">
+      <c r="G10" s="62" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="24" t="s">
@@ -1403,14 +1255,14 @@
       <c r="A11" s="4">
         <v>2</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="43"/>
+      <c r="C11" s="38"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
       <c r="H11" s="24" t="s">
         <v>19</v>
       </c>
@@ -1421,17 +1273,17 @@
       <c r="M11" s="17"/>
     </row>
     <row r="12" spans="1:13" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="49"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="52"/>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
       <c r="L12" s="17"/>
@@ -1441,16 +1293,16 @@
       <c r="A13" s="4">
         <v>1</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="50"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="51" t="s">
+      <c r="F13" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="52" t="s">
+      <c r="G13" s="54" t="s">
         <v>16</v>
       </c>
       <c r="H13" s="24" t="s">
@@ -1466,14 +1318,14 @@
       <c r="A14" s="4">
         <v>2</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="50"/>
+      <c r="C14" s="42"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="52"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="54"/>
       <c r="H14" s="24" t="s">
         <v>22</v>
       </c>
@@ -1487,14 +1339,14 @@
       <c r="A15" s="4">
         <v>3</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="54"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="52"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="54"/>
       <c r="H15" s="24" t="s">
         <v>22</v>
       </c>
@@ -1508,14 +1360,14 @@
       <c r="A16" s="4">
         <v>4</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="54"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="52"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="54"/>
       <c r="H16" s="24" t="s">
         <v>22</v>
       </c>
@@ -1529,10 +1381,10 @@
       <c r="A17" s="4">
         <v>5</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="50"/>
+      <c r="C17" s="42"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4">
@@ -1569,10 +1421,10 @@
       <c r="A19" s="4">
         <v>1</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="43"/>
+      <c r="C19" s="38"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4">
@@ -1592,10 +1444,10 @@
       <c r="A20" s="4">
         <v>2</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="43"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4">
@@ -1615,10 +1467,10 @@
       <c r="A21" s="4">
         <v>3</v>
       </c>
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="43"/>
+      <c r="C21" s="38"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4">
@@ -1638,10 +1490,10 @@
       <c r="A22" s="4">
         <v>4</v>
       </c>
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="43"/>
+      <c r="C22" s="38"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4">
@@ -1661,10 +1513,10 @@
       <c r="A23" s="4">
         <v>5</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="43"/>
+      <c r="C23" s="38"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4">
@@ -1684,10 +1536,10 @@
       <c r="A24" s="4">
         <v>6</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="43"/>
+      <c r="C24" s="38"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4">
@@ -1707,10 +1559,10 @@
       <c r="A25" s="4">
         <v>7</v>
       </c>
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="43"/>
+      <c r="C25" s="38"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4">
@@ -1730,10 +1582,10 @@
       <c r="A26" s="4">
         <v>8</v>
       </c>
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="43"/>
+      <c r="C26" s="38"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4">
@@ -1753,10 +1605,10 @@
       <c r="A27" s="4">
         <v>9</v>
       </c>
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="54"/>
+      <c r="C27" s="40"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4">
@@ -1776,10 +1628,10 @@
       <c r="A28" s="4">
         <v>10</v>
       </c>
-      <c r="B28" s="53" t="s">
+      <c r="B28" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="54"/>
+      <c r="C28" s="40"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4">
@@ -1799,10 +1651,10 @@
       <c r="A29" s="4">
         <v>11</v>
       </c>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="43"/>
+      <c r="C29" s="38"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4">
@@ -1822,10 +1674,10 @@
       <c r="A30" s="4">
         <v>12</v>
       </c>
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="50"/>
+      <c r="C30" s="42"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4">
@@ -1842,11 +1694,11 @@
       <c r="M30" s="17"/>
     </row>
     <row r="31" spans="1:13" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="65" t="s">
+      <c r="A31" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="67"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="45"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
       <c r="F31" s="6">
@@ -1861,15 +1713,15 @@
       <c r="M31" s="17"/>
     </row>
     <row r="32" spans="1:13" s="9" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="68" t="s">
+      <c r="A32" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="61"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="36"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
       <c r="J32" s="17"/>
@@ -1878,9 +1730,11 @@
       <c r="M32" s="23"/>
     </row>
     <row r="33" spans="1:13" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A33" s="17"/>
+      <c r="A33" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="B33" s="17" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
@@ -1895,9 +1749,11 @@
       <c r="M33" s="17"/>
     </row>
     <row r="34" spans="1:13" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A34" s="17"/>
+      <c r="A34" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="B34" s="17" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
@@ -1912,9 +1768,11 @@
       <c r="M34" s="17"/>
     </row>
     <row r="35" spans="1:13" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A35" s="17"/>
+      <c r="A35" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="B35" s="17" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
@@ -1929,18 +1787,16 @@
       <c r="M35" s="17"/>
     </row>
     <row r="36" spans="1:13" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A36" s="17"/>
-      <c r="B36" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" s="63"/>
+      <c r="A36" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="41"/>
+      <c r="C36" s="41"/>
       <c r="D36" s="17"/>
       <c r="E36" s="17"/>
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
-      <c r="H36" s="27" t="s">
-        <v>70</v>
-      </c>
+      <c r="H36" s="27"/>
       <c r="I36" s="17"/>
       <c r="J36" s="17"/>
       <c r="K36" s="17"/>
@@ -1948,10 +1804,10 @@
       <c r="M36" s="17"/>
     </row>
     <row r="37" spans="1:13" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A37" s="17"/>
-      <c r="B37" s="17" t="s">
-        <v>67</v>
-      </c>
+      <c r="A37" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="17"/>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
       <c r="E37" s="17"/>
@@ -1965,10 +1821,10 @@
       <c r="M37" s="17"/>
     </row>
     <row r="38" spans="1:13" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17" t="s">
-        <v>67</v>
-      </c>
+      <c r="A38" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="17"/>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
@@ -1982,10 +1838,10 @@
       <c r="M38" s="17"/>
     </row>
     <row r="39" spans="1:13" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A39" s="17"/>
-      <c r="B39" s="17" t="s">
-        <v>67</v>
-      </c>
+      <c r="A39" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="17"/>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
       <c r="E39" s="17"/>
@@ -1999,17 +1855,17 @@
       <c r="M39" s="17"/>
     </row>
     <row r="40" spans="1:13" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A40" s="17"/>
-      <c r="B40" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
+      <c r="A40" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="34"/>
       <c r="J40" s="17"/>
       <c r="K40" s="17"/>
       <c r="L40" s="17"/>
@@ -2017,17 +1873,13 @@
     </row>
     <row r="41" spans="1:13" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
-      <c r="B41" s="63" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="63"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
       <c r="D41" s="17"/>
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
       <c r="G41" s="17"/>
-      <c r="H41" s="27" t="s">
-        <v>71</v>
-      </c>
+      <c r="H41" s="27"/>
       <c r="I41" s="17"/>
       <c r="J41" s="17"/>
       <c r="K41" s="17"/>
@@ -2035,9 +1887,7 @@
       <c r="M41" s="17"/>
     </row>
     <row r="42" spans="1:13" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A42" s="17" t="s">
-        <v>67</v>
-      </c>
+      <c r="A42" s="17"/>
       <c r="B42" s="27"/>
       <c r="C42" s="27"/>
       <c r="D42" s="17"/>
@@ -2052,9 +1902,7 @@
       <c r="M42" s="17"/>
     </row>
     <row r="43" spans="1:13" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A43" s="17" t="s">
-        <v>67</v>
-      </c>
+      <c r="A43" s="17"/>
       <c r="B43" s="27"/>
       <c r="C43" s="27"/>
       <c r="D43" s="17"/>
@@ -2069,9 +1917,7 @@
       <c r="M43" s="17"/>
     </row>
     <row r="44" spans="1:13" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A44" s="17" t="s">
-        <v>67</v>
-      </c>
+      <c r="A44" s="17"/>
       <c r="B44" s="27"/>
       <c r="C44" s="27"/>
       <c r="D44" s="17"/>
@@ -2086,9 +1932,7 @@
       <c r="M44" s="17"/>
     </row>
     <row r="45" spans="1:13" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
-        <v>67</v>
-      </c>
+      <c r="A45" s="17"/>
       <c r="B45" s="27"/>
       <c r="C45" s="27"/>
       <c r="D45" s="17"/>
@@ -2103,9 +1947,7 @@
       <c r="M45" s="17"/>
     </row>
     <row r="46" spans="1:13" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A46" s="17" t="s">
-        <v>67</v>
-      </c>
+      <c r="A46" s="17"/>
       <c r="B46" s="27"/>
       <c r="C46" s="27"/>
       <c r="D46" s="17"/>
@@ -2120,9 +1962,7 @@
       <c r="M46" s="17"/>
     </row>
     <row r="47" spans="1:13" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A47" s="17" t="s">
-        <v>67</v>
-      </c>
+      <c r="A47" s="17"/>
       <c r="B47" s="27"/>
       <c r="C47" s="27"/>
       <c r="D47" s="17"/>
@@ -2137,52 +1977,40 @@
       <c r="M47" s="17"/>
     </row>
     <row r="48" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="B48" s="40"/>
-      <c r="C48" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D48" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
-      <c r="I48" s="37" t="s">
-        <v>56</v>
-      </c>
+      <c r="A48" s="34"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="67"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="69"/>
+      <c r="F48" s="69"/>
+      <c r="G48" s="69"/>
+      <c r="H48" s="69"/>
+      <c r="I48" s="66"/>
       <c r="J48" s="17"/>
       <c r="K48" s="17"/>
       <c r="L48" s="17"/>
       <c r="M48" s="17"/>
     </row>
     <row r="49" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="40"/>
-      <c r="B49" s="40"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="E49" s="64"/>
-      <c r="F49" s="64"/>
-      <c r="G49" s="64"/>
-      <c r="H49" s="64"/>
-      <c r="I49" s="37"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="67"/>
+      <c r="D49" s="69"/>
+      <c r="E49" s="69"/>
+      <c r="F49" s="69"/>
+      <c r="G49" s="69"/>
+      <c r="H49" s="69"/>
+      <c r="I49" s="66"/>
       <c r="J49" s="17"/>
       <c r="K49" s="17"/>
       <c r="L49" s="17"/>
       <c r="M49" s="17"/>
     </row>
     <row r="50" spans="1:13" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A50" s="17" t="s">
-        <v>67</v>
-      </c>
+      <c r="A50" s="17"/>
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
-      <c r="D50" s="31"/>
+      <c r="D50" s="30"/>
       <c r="E50" s="17"/>
       <c r="F50" s="17"/>
       <c r="G50" s="17"/>
@@ -2194,56 +2022,44 @@
       <c r="M50" s="17"/>
     </row>
     <row r="51" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="B51" s="40"/>
-      <c r="C51" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D51" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="E51" s="39"/>
-      <c r="F51" s="39"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="39"/>
-      <c r="I51" s="37" t="s">
-        <v>56</v>
-      </c>
+      <c r="A51" s="34"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="67"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="69"/>
+      <c r="G51" s="69"/>
+      <c r="H51" s="69"/>
+      <c r="I51" s="66"/>
       <c r="J51" s="17"/>
       <c r="K51" s="17"/>
       <c r="L51" s="17"/>
       <c r="M51" s="17"/>
     </row>
     <row r="52" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="40"/>
-      <c r="B52" s="40"/>
-      <c r="C52" s="38"/>
-      <c r="D52" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="E52" s="64"/>
-      <c r="F52" s="64"/>
-      <c r="G52" s="64"/>
-      <c r="H52" s="64"/>
-      <c r="I52" s="37"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="67"/>
+      <c r="D52" s="69"/>
+      <c r="E52" s="69"/>
+      <c r="F52" s="69"/>
+      <c r="G52" s="69"/>
+      <c r="H52" s="69"/>
+      <c r="I52" s="66"/>
       <c r="J52" s="17"/>
       <c r="K52" s="17"/>
       <c r="L52" s="17"/>
       <c r="M52" s="17"/>
     </row>
     <row r="53" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="28" t="s">
-        <v>67</v>
-      </c>
+      <c r="A53" s="28"/>
       <c r="B53" s="29"/>
       <c r="C53" s="28"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="30"/>
-      <c r="H53" s="30"/>
+      <c r="D53" s="70"/>
+      <c r="E53" s="71"/>
+      <c r="F53" s="71"/>
+      <c r="G53" s="71"/>
+      <c r="H53" s="71"/>
       <c r="I53" s="17"/>
       <c r="J53" s="17"/>
       <c r="K53" s="17"/>
@@ -2253,16 +2069,12 @@
     <row r="54" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="28"/>
       <c r="B54" s="29"/>
-      <c r="C54" s="71" t="s">
-        <v>58</v>
-      </c>
-      <c r="D54" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="E54" s="39"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="39"/>
+      <c r="C54" s="68"/>
+      <c r="D54" s="69"/>
+      <c r="E54" s="69"/>
+      <c r="F54" s="69"/>
+      <c r="G54" s="69"/>
+      <c r="H54" s="69"/>
       <c r="I54" s="17"/>
       <c r="J54" s="17"/>
       <c r="K54" s="17"/>
@@ -2270,18 +2082,14 @@
       <c r="M54" s="17"/>
     </row>
     <row r="55" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="17" t="s">
-        <v>67</v>
-      </c>
+      <c r="A55" s="17"/>
       <c r="B55" s="17"/>
-      <c r="C55" s="71"/>
-      <c r="D55" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="E55" s="40"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="40"/>
+      <c r="C55" s="68"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="34"/>
+      <c r="H55" s="34"/>
       <c r="I55" s="17"/>
       <c r="J55" s="17"/>
       <c r="K55" s="17"/>
@@ -2289,9 +2097,7 @@
       <c r="M55" s="17"/>
     </row>
     <row r="56" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="17" t="s">
-        <v>77</v>
-      </c>
+      <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="17"/>
       <c r="D56" s="17"/>
@@ -2306,9 +2112,7 @@
       <c r="M56" s="17"/>
     </row>
     <row r="57" spans="1:13" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="17" t="s">
-        <v>77</v>
-      </c>
+      <c r="A57" s="17"/>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
@@ -2323,9 +2127,7 @@
       <c r="M57" s="17"/>
     </row>
     <row r="58" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="17" t="s">
-        <v>77</v>
-      </c>
+      <c r="A58" s="17"/>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
@@ -2340,26 +2142,22 @@
       <c r="M58" s="17"/>
     </row>
     <row r="59" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="62" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59" s="62"/>
-      <c r="C59" s="62"/>
-      <c r="D59" s="62"/>
-      <c r="E59" s="62"/>
-      <c r="F59" s="62"/>
-      <c r="G59" s="62"/>
-      <c r="H59" s="62"/>
-      <c r="I59" s="62"/>
+      <c r="A59" s="37"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
       <c r="J59" s="17"/>
       <c r="K59" s="17"/>
       <c r="L59" s="17"/>
       <c r="M59" s="17"/>
     </row>
     <row r="60" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="17" t="s">
-        <v>77</v>
-      </c>
+      <c r="A60" s="17"/>
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
@@ -2374,20 +2172,14 @@
       <c r="M60" s="17"/>
     </row>
     <row r="61" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="B61" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="C61" s="62"/>
+      <c r="A61" s="17"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
       <c r="D61" s="10"/>
       <c r="E61" s="10"/>
       <c r="F61" s="11"/>
       <c r="G61" s="10"/>
-      <c r="H61" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="H61" s="11"/>
       <c r="I61" s="10"/>
       <c r="J61" s="17"/>
       <c r="K61" s="17"/>
@@ -2395,9 +2187,7 @@
       <c r="M61" s="17"/>
     </row>
     <row r="62" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="17" t="s">
-        <v>77</v>
-      </c>
+      <c r="A62" s="17"/>
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
@@ -2412,9 +2202,7 @@
       <c r="M62" s="17"/>
     </row>
     <row r="63" spans="1:13" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="17" t="s">
-        <v>77</v>
-      </c>
+      <c r="A63" s="17"/>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
@@ -2429,9 +2217,7 @@
       <c r="M63" s="17"/>
     </row>
     <row r="64" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="17" t="s">
-        <v>77</v>
-      </c>
+      <c r="A64" s="17"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
@@ -2446,9 +2232,7 @@
       <c r="M64" s="17"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A65" s="17" t="s">
-        <v>77</v>
-      </c>
+      <c r="A65" s="17"/>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
@@ -2463,20 +2247,14 @@
       <c r="M65" s="10"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A66" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="B66" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="C66" s="62"/>
+      <c r="A66" s="17"/>
+      <c r="B66" s="37"/>
+      <c r="C66" s="37"/>
       <c r="D66" s="10"/>
       <c r="E66" s="10"/>
       <c r="F66" s="11"/>
       <c r="G66" s="10"/>
-      <c r="H66" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="H66" s="11"/>
       <c r="I66" s="10"/>
       <c r="J66" s="10"/>
       <c r="K66" s="10"/>
@@ -2484,9 +2262,7 @@
       <c r="M66" s="10"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A67" s="17" t="s">
-        <v>77</v>
-      </c>
+      <c r="A67" s="17"/>
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
       <c r="D67" s="10"/>
@@ -2501,9 +2277,7 @@
       <c r="M67" s="10"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A68" s="17" t="s">
-        <v>77</v>
-      </c>
+      <c r="A68" s="17"/>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
       <c r="D68" s="10"/>
@@ -2518,15 +2292,13 @@
       <c r="M68" s="10"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A69" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="B69" s="34"/>
-      <c r="C69" s="34"/>
-      <c r="D69" s="34"/>
-      <c r="E69" s="34"/>
-      <c r="F69" s="35"/>
-      <c r="G69" s="34"/>
+      <c r="A69" s="32"/>
+      <c r="B69" s="32"/>
+      <c r="C69" s="32"/>
+      <c r="D69" s="32"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="33"/>
+      <c r="G69" s="32"/>
       <c r="H69" s="10"/>
       <c r="I69" s="10"/>
       <c r="J69" s="10"/>
@@ -2535,15 +2307,13 @@
       <c r="M69" s="10"/>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A70" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="B70" s="36"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="36"/>
-      <c r="F70" s="36"/>
-      <c r="G70" s="36"/>
+      <c r="A70" s="65"/>
+      <c r="B70" s="65"/>
+      <c r="C70" s="65"/>
+      <c r="D70" s="65"/>
+      <c r="E70" s="65"/>
+      <c r="F70" s="65"/>
+      <c r="G70" s="65"/>
       <c r="H70" s="10"/>
       <c r="I70" s="10"/>
       <c r="J70" s="10"/>
@@ -2552,15 +2322,13 @@
       <c r="M70" s="10"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A71" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="B71" s="36"/>
-      <c r="C71" s="36"/>
-      <c r="D71" s="36"/>
-      <c r="E71" s="36"/>
-      <c r="F71" s="36"/>
-      <c r="G71" s="36"/>
+      <c r="A71" s="65"/>
+      <c r="B71" s="65"/>
+      <c r="C71" s="65"/>
+      <c r="D71" s="65"/>
+      <c r="E71" s="65"/>
+      <c r="F71" s="65"/>
+      <c r="G71" s="65"/>
       <c r="H71" s="10"/>
       <c r="I71" s="10"/>
       <c r="J71" s="10"/>
@@ -2569,7 +2337,50 @@
       <c r="M71" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="58">
+  <mergeCells count="59">
+    <mergeCell ref="A70:G70"/>
+    <mergeCell ref="A71:G71"/>
+    <mergeCell ref="I48:I49"/>
+    <mergeCell ref="I51:I52"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:H48"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:H51"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:H54"/>
+    <mergeCell ref="D55:H55"/>
+    <mergeCell ref="A48:B49"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D52:H52"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:F16"/>
+    <mergeCell ref="G13:G16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A18:I18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="A40:I40"/>
     <mergeCell ref="A51:B52"/>
     <mergeCell ref="F32:G32"/>
     <mergeCell ref="A59:I59"/>
@@ -2586,48 +2397,6 @@
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A32:E32"/>
-    <mergeCell ref="D52:H52"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:F16"/>
-    <mergeCell ref="G13:G16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A18:I18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A70:G70"/>
-    <mergeCell ref="A71:G71"/>
-    <mergeCell ref="I48:I49"/>
-    <mergeCell ref="I51:I52"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:H48"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:H51"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:H54"/>
-    <mergeCell ref="D55:H55"/>
-    <mergeCell ref="A48:B49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>